<commit_message>
Fully functional. All major requirements has been implemented. Now MongoDB Connection is adding...
</commit_message>
<xml_diff>
--- a/Invoiceasy/Libs/Files/CoreFiles/TemplateFiles/challan-template.xlsx
+++ b/Invoiceasy/Libs/Files/CoreFiles/TemplateFiles/challan-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzsmu\OneDrive\Desktop\MzsWorkSpace-2020\Moni-Org-IC-Project\Moni-Org-IC-Project-Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzsmu\source\repos\Invoiceasy\Invoiceasy\Libs\Files\CoreFiles\TemplateFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_5A11C5309897ECB85CEE23C6D348B8468920EF35" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CAFB5BF2-A10F-425C-B17E-531CB9AB1D86}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055BE73B-6CEA-4657-9357-B81CC6A4D522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t xml:space="preserve">                        IT</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
     <t>Total Quantity:</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   <si>
     <t>Reg. Office: Nishat Nagar, Diabari, Turag, Dhaka - 1230, T: +880 9638 016 900, E: info@theunytd.com, W: www.theunytd.com
 Dhaka Office: 273, Shah Kabir Mazar Road, Azampur, Uttara, Dhaka, Bangladesh.</t>
+  </si>
+  <si>
+    <t>Note:</t>
   </si>
 </sst>
 </file>
@@ -544,6 +544,33 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -611,33 +638,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1294,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:E9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,29 +1321,29 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="62" t="s">
+      <c r="E2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:7" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:7" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
@@ -1354,7 +1354,7 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="41" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
@@ -1365,72 +1365,72 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64"/>
-      <c r="B7" s="65" t="s">
+      <c r="A7" s="41"/>
+      <c r="B7" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
     </row>
     <row r="8" spans="1:7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
       <c r="F8" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" customFormat="1" ht="31.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="64"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="64"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="14"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="64"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="16"/>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="70"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="17" t="s">
         <v>11</v>
       </c>
@@ -1439,7 +1439,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="64"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
@@ -1448,7 +1448,7 @@
       <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
@@ -1457,7 +1457,7 @@
       <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="51" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="18"/>
@@ -1468,7 +1468,7 @@
       <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
@@ -1476,7 +1476,7 @@
       <c r="G16" s="24"/>
     </row>
     <row r="17" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
       <c r="D17" s="20"/>
@@ -1485,7 +1485,7 @@
       <c r="G17" s="23"/>
     </row>
     <row r="18" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
@@ -1494,7 +1494,7 @@
       <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
       <c r="D19" s="20"/>
@@ -1503,7 +1503,7 @@
       <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="51"/>
       <c r="B20" s="18"/>
       <c r="C20" s="27"/>
       <c r="D20" s="20"/>
@@ -1512,7 +1512,7 @@
       <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="51"/>
       <c r="B21" s="18"/>
       <c r="C21" s="27"/>
       <c r="D21" s="20"/>
@@ -1521,7 +1521,7 @@
       <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="18"/>
       <c r="C22" s="27"/>
       <c r="D22" s="20"/>
@@ -1530,7 +1530,7 @@
       <c r="G22" s="26"/>
     </row>
     <row r="23" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="18"/>
       <c r="C23" s="27"/>
       <c r="D23" s="20"/>
@@ -1539,7 +1539,7 @@
       <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="18"/>
       <c r="C24" s="27"/>
       <c r="D24" s="20"/>
@@ -1548,7 +1548,7 @@
       <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="18"/>
       <c r="C25" s="27"/>
       <c r="D25" s="20"/>
@@ -1557,7 +1557,7 @@
       <c r="G25" s="26"/>
     </row>
     <row r="26" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="18"/>
       <c r="C26" s="27"/>
       <c r="D26" s="20"/>
@@ -1566,7 +1566,7 @@
       <c r="G26" s="26"/>
     </row>
     <row r="27" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="51"/>
       <c r="B27" s="18"/>
       <c r="C27" s="27"/>
       <c r="D27" s="20"/>
@@ -1575,7 +1575,7 @@
       <c r="G27" s="26"/>
     </row>
     <row r="28" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="52" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="18"/>
@@ -1586,7 +1586,7 @@
       <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="43"/>
+      <c r="A29" s="52"/>
       <c r="B29" s="18"/>
       <c r="C29" s="27"/>
       <c r="D29" s="20"/>
@@ -1595,7 +1595,7 @@
       <c r="G29" s="26"/>
     </row>
     <row r="30" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="43"/>
+      <c r="A30" s="52"/>
       <c r="B30" s="18"/>
       <c r="C30" s="27"/>
       <c r="D30" s="20"/>
@@ -1604,7 +1604,7 @@
       <c r="G30" s="26"/>
     </row>
     <row r="31" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
+      <c r="A31" s="52"/>
       <c r="B31" s="18"/>
       <c r="C31" s="27"/>
       <c r="D31" s="20"/>
@@ -1613,7 +1613,7 @@
       <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
+      <c r="A32" s="52"/>
       <c r="B32" s="18"/>
       <c r="C32" s="27"/>
       <c r="D32" s="28"/>
@@ -1622,7 +1622,7 @@
       <c r="G32" s="26"/>
     </row>
     <row r="33" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
+      <c r="A33" s="52"/>
       <c r="B33" s="18"/>
       <c r="C33" s="27"/>
       <c r="D33" s="28"/>
@@ -1631,7 +1631,7 @@
       <c r="G33" s="26"/>
     </row>
     <row r="34" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
+      <c r="A34" s="52"/>
       <c r="B34" s="18"/>
       <c r="C34" s="27"/>
       <c r="D34" s="28"/>
@@ -1640,7 +1640,7 @@
       <c r="G34" s="26"/>
     </row>
     <row r="35" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
+      <c r="A35" s="52"/>
       <c r="B35" s="18"/>
       <c r="C35" s="27"/>
       <c r="D35" s="21"/>
@@ -1649,7 +1649,7 @@
       <c r="G35" s="29"/>
     </row>
     <row r="36" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
+      <c r="A36" s="52"/>
       <c r="B36" s="18"/>
       <c r="C36" s="28"/>
       <c r="D36" s="28"/>
@@ -1658,7 +1658,7 @@
       <c r="G36" s="29"/>
     </row>
     <row r="37" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
+      <c r="A37" s="52"/>
       <c r="B37" s="18"/>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
@@ -1667,7 +1667,7 @@
       <c r="G37" s="29"/>
     </row>
     <row r="38" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
+      <c r="A38" s="52"/>
       <c r="B38" s="18"/>
       <c r="C38" s="28"/>
       <c r="D38" s="28"/>
@@ -1676,7 +1676,7 @@
       <c r="G38" s="29"/>
     </row>
     <row r="39" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
+      <c r="A39" s="52"/>
       <c r="B39" s="18"/>
       <c r="C39" s="28"/>
       <c r="D39" s="28"/>
@@ -1685,61 +1685,58 @@
       <c r="G39" s="29"/>
     </row>
     <row r="40" spans="1:7" s="13" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
+      <c r="A40" s="53" t="s">
         <v>15</v>
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="28"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
       <c r="F40" s="30"/>
       <c r="G40" s="30"/>
     </row>
     <row r="41" spans="1:7" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
-      <c r="B41" s="47" t="s">
+      <c r="A41" s="53"/>
+      <c r="B41" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="57"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="48"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="F41" s="56"/>
-      <c r="G41" s="31">
-        <f>SUM(G13:G40)</f>
-        <v>0</v>
-      </c>
+      <c r="F41" s="65"/>
+      <c r="G41" s="31"/>
     </row>
     <row r="42" spans="1:7" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="57"/>
+      <c r="A42" s="53"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="66"/>
       <c r="G42" s="32"/>
     </row>
     <row r="43" spans="1:7" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="58"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
       <c r="G43" s="32"/>
     </row>
     <row r="44" spans="1:7" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
+      <c r="A44" s="53"/>
       <c r="B44" s="33"/>
-      <c r="C44" s="59"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
-      <c r="F44" s="60"/>
-      <c r="G44" s="60"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
+      <c r="G44" s="69"/>
     </row>
     <row r="45" spans="1:7" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
+      <c r="A45" s="53"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
@@ -1748,29 +1745,29 @@
       <c r="G45" s="35"/>
     </row>
     <row r="46" spans="1:7" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
+      <c r="A46" s="53"/>
       <c r="B46" s="36"/>
       <c r="C46" s="36"/>
       <c r="D46" s="14"/>
       <c r="E46" s="34"/>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
+      <c r="F46" s="70"/>
+      <c r="G46" s="70"/>
     </row>
     <row r="47" spans="1:7" s="13" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" s="39"/>
+      <c r="A47" s="53"/>
+      <c r="B47" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="48"/>
       <c r="D47" s="14"/>
       <c r="E47" s="34"/>
-      <c r="F47" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="G47" s="39"/>
+      <c r="F47" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="48"/>
     </row>
     <row r="48" spans="1:7" s="13" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="45"/>
+      <c r="A48" s="54"/>
       <c r="B48" s="14"/>
       <c r="C48" s="37"/>
       <c r="D48" s="38"/>
@@ -1779,27 +1776,18 @@
       <c r="G48" s="35"/>
     </row>
     <row r="49" spans="1:7" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="41"/>
+      <c r="A49" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E2:G3"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="A6:A14"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="F47:G47"/>
     <mergeCell ref="A49:G49"/>
@@ -1813,6 +1801,15 @@
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="C44:G44"/>
     <mergeCell ref="F46:G46"/>
+    <mergeCell ref="E2:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="A6:A14"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="5" scale="92" orientation="portrait" r:id="rId1"/>

</xml_diff>